<commit_message>
Added supplemental oxygen to respiratory methodology, including validation.
</commit_message>
<xml_diff>
--- a/test/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/test/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E79F8B6-3D03-49BA-948E-DAECF2377C25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="525" windowWidth="15045" windowHeight="7620" tabRatio="643" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="28410" yWindow="3630" windowWidth="25845" windowHeight="22755" tabRatio="643" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -17,6 +23,7 @@
     <sheet name="MainstemIntubation" sheetId="19" r:id="rId8"/>
     <sheet name="EsophagealIntubation" sheetId="24" r:id="rId9"/>
     <sheet name="Apnea" sheetId="45" r:id="rId10"/>
+    <sheet name="Supplemental Oxygen" sheetId="46" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">AirwayObstructionVaried!#REF!</definedName>
@@ -28,12 +35,20 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">MainstemIntubation!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$17</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="263">
   <si>
     <t>Oxygen Saturation</t>
   </si>
@@ -777,12 +792,57 @@
   </si>
   <si>
     <t>Apnea: Severity = 1.0</t>
+  </si>
+  <si>
+    <t>Nasal Cannala</t>
+  </si>
+  <si>
+    <t>SupplementalOxygen: Nasal Cannula</t>
+  </si>
+  <si>
+    <t>Default flow = 3.5 L/min</t>
+  </si>
+  <si>
+    <t>Fraction of Inspired Oxygen (FiO2)</t>
+  </si>
+  <si>
+    <t>Increase to ~0.4 @cite korupolu2009early, @cite bailey2007early</t>
+  </si>
+  <si>
+    <t>Increase to ~0.5 @cite korupolu2009early, @cite bailey2007early</t>
+  </si>
+  <si>
+    <t>Increase to ~0.9 @cite korupolu2009early, @cite bailey2007early</t>
+  </si>
+  <si>
+    <t>Simple Mask</t>
+  </si>
+  <si>
+    <t>Non-Rebreather Mask</t>
+  </si>
+  <si>
+    <t>Supplemental Oxygen</t>
+  </si>
+  <si>
+    <t>Nasal cannula, simple mask, and non-rebreather mask</t>
+  </si>
+  <si>
+    <t>SupplementalOxygen: Simple Mask</t>
+  </si>
+  <si>
+    <t>SupplementalOxygen: Non-Rebreather Mask</t>
+  </si>
+  <si>
+    <t>Default flow = 7.5 L/min</t>
+  </si>
+  <si>
+    <t>Default flow = 10.0 L/min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1619,6 +1679,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1666,7 +1729,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1699,9 +1762,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1734,6 +1814,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1909,14 +2006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K19"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,19 +2399,19 @@
         <v>110</v>
       </c>
       <c r="F11" s="29">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>113</v>
       </c>
       <c r="H11" s="30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>114</v>
       </c>
       <c r="J11" s="31">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>111</v>
@@ -2337,19 +2434,19 @@
         <v>110</v>
       </c>
       <c r="F12" s="29">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>113</v>
       </c>
       <c r="H12" s="30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>114</v>
       </c>
       <c r="J12" s="31">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>111</v>
@@ -2569,35 +2666,70 @@
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="27" t="s">
+        <v>257</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>220</v>
+      <c r="D19" s="28" t="s">
+        <v>258</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>110</v>
       </c>
       <c r="F19" s="29">
-        <f>SUM(F3:F18)</f>
-        <v>239</v>
+        <v>3</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>113</v>
       </c>
       <c r="H19" s="30">
-        <f>SUM(H3:H18)</f>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>114</v>
       </c>
       <c r="J19" s="31">
-        <f>SUM(J3:J18)</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="29">
+        <f>SUM(F3:F19)</f>
+        <v>258</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="30">
+        <f>SUM(H3:H19)</f>
+        <v>28</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="31">
+        <f>SUM(J3:J19)</f>
+        <v>27</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2612,10 +2744,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2919,8 +3051,367 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA568C8-ADAE-4E7B-960D-973F34ED96D5}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="A12:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="8">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="8">
+        <v>330</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="8">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="8">
+        <v>330</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="8">
+        <v>30</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="8">
+        <v>330</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4026,7 +4517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4613,7 +5104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5436,11 +5927,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,7 +5967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -5804,9 +6295,9 @@
         <v>142</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>143</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -5816,9 +6307,9 @@
         <v>143</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T6" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T6" s="9" t="s">
         <v>143</v>
       </c>
       <c r="U6" s="3" t="s">
@@ -5875,21 +6366,21 @@
         <v>146</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P7" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="9" t="s">
         <v>147</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="R7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="R7" s="18" t="s">
         <v>147</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T7" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T7" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U7" s="3" t="s">
@@ -6005,9 +6496,9 @@
         <v>153</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>153</v>
       </c>
       <c r="M9" s="3" t="s">
@@ -6017,21 +6508,21 @@
         <v>153</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="P9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>154</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="R9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="R9" s="9" t="s">
         <v>154</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="T9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="T9" s="9" t="s">
         <v>154</v>
       </c>
       <c r="U9" s="3" t="s">
@@ -6377,9 +6868,9 @@
         <v>156</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P16" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="P16" s="9" t="s">
         <v>157</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -6389,9 +6880,9 @@
         <v>143</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T16" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T16" s="9" t="s">
         <v>143</v>
       </c>
       <c r="U16" s="3" t="s">
@@ -6448,21 +6939,21 @@
         <v>158</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P17" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="P17" s="9" t="s">
         <v>159</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="R17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="R17" s="18" t="s">
         <v>159</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T17" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T17" s="9" t="s">
         <v>159</v>
       </c>
       <c r="U17" s="3" t="s">
@@ -6507,9 +6998,9 @@
         <v>161</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L18" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>153</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -6519,21 +7010,21 @@
         <v>162</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="P18" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="P18" s="9" t="s">
         <v>154</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="R18" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="R18" s="9" t="s">
         <v>154</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="T18" s="18" t="s">
+      <c r="T18" s="9" t="s">
         <v>154</v>
       </c>
       <c r="U18" s="3" t="s">
@@ -6990,7 +7481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7507,7 +7998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8024,14 +8515,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8485,7 +8976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Updates to Pulmonary Fibrosis for combined effects. Added Pulmonary Fibrosis scenario and updated validation. Removed erroneous link.
</commit_message>
<xml_diff>
--- a/test/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/test/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anusham2\Desktop\Engine\test\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_UIUC\source\test\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A74002-D867-4BDA-BFAD-97FB95A42B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15165" yWindow="7050" windowWidth="32670" windowHeight="23535" tabRatio="643" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="27195" yWindow="8490" windowWidth="25335" windowHeight="16005" tabRatio="643" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -35,7 +36,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">MainstemIntubation!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$17</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -860,12 +861,6 @@
     <t>Decreases</t>
   </si>
   <si>
-    <t>Increase,  Tachypnea, Dypsnea,  &gt; 30 @cite gunning2003pathophysiology</t>
-  </si>
-  <si>
-    <t>&lt; 60% of normal @cite nava1999IPF,gunning2003pathophysiology</t>
-  </si>
-  <si>
     <t xml:space="preserve">Increase, Pulmonary Hypertension, &gt; 140 mm Hg @cite ganeshraghu2015pulmhypertensioninipf </t>
   </si>
   <si>
@@ -879,12 +874,18 @@
   </si>
   <si>
     <t xml:space="preserve">Decrease </t>
+  </si>
+  <si>
+    <t>Dyspnea, &lt; 60% of normal @cite nava1999IPF, @cite gunning2003pathophysiology</t>
+  </si>
+  <si>
+    <t>Increase,  Tachypnea,   &gt; 30 @cite gunning2003pathophysiology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1804,6 +1805,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1839,6 +1857,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2014,7 +2049,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2752,7 +2787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3060,7 +3095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3419,11 +3454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,20 +3468,23 @@
     <col min="3" max="3" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
     <col min="11" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" customWidth="1"/>
     <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
     <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
     <col min="17" max="17" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.140625" customWidth="1"/>
     <col min="19" max="19" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="20" max="20" width="28.140625" customWidth="1"/>
     <col min="21" max="21" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1"/>
+    <col min="22" max="22" width="28.140625" customWidth="1"/>
     <col min="23" max="23" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.140625" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3609,7 +3647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
@@ -3635,16 +3673,16 @@
         <v>269</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>270</v>
+        <v>107</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>271</v>
+        <v>107</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>109</v>
@@ -3656,31 +3694,31 @@
         <v>111</v>
       </c>
       <c r="P4" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="T4" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>110</v>
       </c>
       <c r="V4" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>109</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>108</v>
@@ -3692,7 +3730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4798,7 +4836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5385,7 +5423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6208,7 +6246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -7762,7 +7800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8279,7 +8317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8796,7 +8834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9257,7 +9295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Added pulmonary fibrosis descriptions to respiratory methodology report. Validation table formating fix.
</commit_message>
<xml_diff>
--- a/test/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/test/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_Documentation\source\test\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B4CF3B-0B7C-4B71-8291-E7211322C7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B8DD8E-E1C5-457F-86E1-A7C7E2882E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1695" windowWidth="40350" windowHeight="25635" tabRatio="643" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14055" yWindow="5250" windowWidth="30495" windowHeight="24645" tabRatio="643" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -5380,8 +5380,8 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y14" sqref="A12:Y14"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6200,35 +6200,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y4" sqref="A2:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.140625" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.140625" customWidth="1"/>
-    <col min="19" max="19" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.140625" customWidth="1"/>
-    <col min="21" max="21" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.140625" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.140625" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6416,13 +6417,13 @@
         <v>246</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>251</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>258</v>
@@ -6477,7 +6478,7 @@
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W18" sqref="A12:W18"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>